<commit_message>
Add process different datatypes isinstance
</commit_message>
<xml_diff>
--- a/my_file.xlsx
+++ b/my_file.xlsx
@@ -55,7 +55,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,12 +85,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,11 +153,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -187,7 +181,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -236,7 +230,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>9.99</v>
+        <v>9.99999</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>5</v>
@@ -246,7 +240,7 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="false">B3*C3</f>
-        <v>49.95</v>
+        <v>49.99995</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,7 +303,7 @@
       </c>
       <c r="B7" s="1" t="n">
         <f aca="false">SUM(B2:B6)</f>
-        <v>49.95</v>
+        <v>49.95999</v>
       </c>
       <c r="C7" s="1" t="n">
         <f aca="false">SUM(C2:C6)</f>
@@ -320,7 +314,7 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="false">SUM(E2:E6)</f>
-        <v>164.83</v>
+        <v>164.87995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>